<commit_message>
Changed LDO to one that has 15V VIn max. Still need to updated caps on either side to be bigger.
</commit_message>
<xml_diff>
--- a/mini/v17/Fubarino_Mini_v17_BOM_Microchip.xlsx
+++ b/mini/v17/Fubarino_Mini_v17_BOM_Microchip.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Brian\fubarino.github.com\mini\v17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0894A127-621C-412B-9ED4-76FFFD86A74F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23925" windowHeight="12045"/>
   </bookViews>
@@ -16,7 +15,7 @@
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
     <sheet name="Project Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -372,31 +371,31 @@
     <t>Toshiba Semiconductor and Storage</t>
   </si>
   <si>
-    <t>AP7215-33YG-13DICT-ND</t>
-  </si>
-  <si>
     <t>Diodes Incorporated</t>
   </si>
   <si>
-    <t>AP7215-33YG-13</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 3.3V 600MA SOT89-3</t>
-  </si>
-  <si>
     <t>Parts changed from last production build</t>
   </si>
   <si>
     <t>PIC32MX270F256D-50I/ML  </t>
+  </si>
+  <si>
+    <t>AZ1117CR2-3.3TRG1-ND</t>
+  </si>
+  <si>
+    <t>AZ1117CR2-3.3TRG1</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 800MA SOT89</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -875,7 +874,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="131">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1033,13 +1032,13 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1082,7 +1081,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1128,32 +1127,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1193,6 +1170,29 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="7" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1202,11 +1202,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1310,23 +1305,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1362,23 +1340,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1560,8 +1521,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1624,8 +1585,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="89"/>
+      <c r="K3" s="123"/>
+      <c r="L3" s="120"/>
       <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
@@ -1641,8 +1602,8 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="90"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="121"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1">
@@ -1658,8 +1619,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="90"/>
+      <c r="K5" s="124"/>
+      <c r="L5" s="121"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1">
@@ -1675,8 +1636,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="90"/>
+      <c r="K6" s="124"/>
+      <c r="L6" s="121"/>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
@@ -1688,8 +1649,8 @@
       <c r="H7" s="45"/>
       <c r="I7" s="59"/>
       <c r="J7" s="85"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="91"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="122"/>
       <c r="M7" s="60"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
@@ -1780,31 +1741,31 @@
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="100">
-        <v>1</v>
-      </c>
-      <c r="D12" s="101" t="s">
+      <c r="C12" s="92">
+        <v>1</v>
+      </c>
+      <c r="D12" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="102" t="s">
+      <c r="E12" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="101" t="s">
+      <c r="F12" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="103" t="s">
+      <c r="G12" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="H12" s="104" t="s">
+      <c r="H12" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="105" t="s">
+      <c r="I12" s="97" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="106" t="s">
+      <c r="J12" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="107">
+      <c r="K12" s="99">
         <v>1</v>
       </c>
       <c r="L12" s="53">
@@ -1819,31 +1780,31 @@
       <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="100">
-        <v>1</v>
-      </c>
-      <c r="D13" s="108" t="s">
+      <c r="C13" s="92">
+        <v>1</v>
+      </c>
+      <c r="D13" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="97" t="s">
+      <c r="E13" s="90" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="101" t="s">
+        <v>116</v>
+      </c>
+      <c r="G13" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="90" t="s">
         <v>119</v>
       </c>
-      <c r="F13" s="109" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13" s="98" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13" s="104" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="96" t="s">
-        <v>116</v>
-      </c>
-      <c r="J13" s="106" t="s">
+      <c r="J13" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="107">
+      <c r="K13" s="99">
         <v>1</v>
       </c>
       <c r="L13" s="53">
@@ -1857,31 +1818,31 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="100">
-        <v>1</v>
-      </c>
-      <c r="D14" s="110" t="s">
+      <c r="C14" s="92">
+        <v>1</v>
+      </c>
+      <c r="D14" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="111" t="s">
+      <c r="E14" s="103" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="112" t="s">
+      <c r="F14" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="113" t="s">
+      <c r="G14" s="105" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="104" t="s">
+      <c r="H14" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="114" t="s">
+      <c r="I14" s="106" t="s">
         <v>83</v>
       </c>
-      <c r="J14" s="106" t="s">
+      <c r="J14" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="107">
+      <c r="K14" s="99">
         <v>1</v>
       </c>
       <c r="L14" s="53">
@@ -1896,31 +1857,31 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="C15" s="100">
+      <c r="C15" s="92">
         <v>2</v>
       </c>
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="115" t="s">
+      <c r="E15" s="107" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="112" t="s">
+      <c r="F15" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="116" t="s">
+      <c r="G15" s="108" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="104" t="s">
+      <c r="H15" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="117" t="s">
+      <c r="I15" s="109" t="s">
         <v>84</v>
       </c>
-      <c r="J15" s="106" t="s">
+      <c r="J15" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="107">
+      <c r="K15" s="99">
         <v>2</v>
       </c>
       <c r="L15" s="53">
@@ -1935,31 +1896,31 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" s="100">
-        <v>1</v>
-      </c>
-      <c r="D16" s="110" t="s">
+      <c r="C16" s="92">
+        <v>1</v>
+      </c>
+      <c r="D16" s="102" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="111" t="s">
+      <c r="E16" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="112" t="s">
+      <c r="F16" s="104" t="s">
         <v>103</v>
       </c>
-      <c r="G16" s="118" t="s">
+      <c r="G16" s="110" t="s">
         <v>104</v>
       </c>
-      <c r="H16" s="104" t="s">
+      <c r="H16" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="119" t="s">
+      <c r="I16" s="111" t="s">
         <v>105</v>
       </c>
-      <c r="J16" s="106" t="s">
+      <c r="J16" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="107">
+      <c r="K16" s="99">
         <v>1</v>
       </c>
       <c r="L16" s="53">
@@ -1974,31 +1935,31 @@
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" s="100">
+      <c r="C17" s="92">
         <v>2</v>
       </c>
-      <c r="D17" s="110" t="s">
+      <c r="D17" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="111" t="s">
+      <c r="E17" s="103" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="112" t="s">
+      <c r="F17" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="113" t="s">
+      <c r="G17" s="105" t="s">
         <v>73</v>
       </c>
-      <c r="H17" s="104" t="s">
+      <c r="H17" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="114" t="s">
+      <c r="I17" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="J17" s="106" t="s">
+      <c r="J17" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="107">
+      <c r="K17" s="99">
         <v>2</v>
       </c>
       <c r="L17" s="53">
@@ -2013,31 +1974,31 @@
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="C18" s="100">
+      <c r="C18" s="92">
         <v>4</v>
       </c>
-      <c r="D18" s="110" t="s">
+      <c r="D18" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="111" t="s">
+      <c r="E18" s="103" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="112" t="s">
+      <c r="F18" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="113" t="s">
+      <c r="G18" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="104" t="s">
+      <c r="H18" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="114" t="s">
+      <c r="I18" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="J18" s="106" t="s">
+      <c r="J18" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="107">
+      <c r="K18" s="99">
         <v>4</v>
       </c>
       <c r="L18" s="53">
@@ -2052,31 +2013,31 @@
       <c r="A19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="100">
-        <v>1</v>
-      </c>
-      <c r="D19" s="110" t="s">
+      <c r="C19" s="92">
+        <v>1</v>
+      </c>
+      <c r="D19" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="120" t="s">
+      <c r="E19" s="112" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="112" t="s">
+      <c r="F19" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="121" t="s">
+      <c r="G19" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="H19" s="104" t="s">
+      <c r="H19" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="122" t="s">
+      <c r="I19" s="114" t="s">
         <v>87</v>
       </c>
-      <c r="J19" s="106" t="s">
+      <c r="J19" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="107">
+      <c r="K19" s="99">
         <v>1</v>
       </c>
       <c r="L19" s="53">
@@ -2091,31 +2052,31 @@
       <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="100">
-        <v>1</v>
-      </c>
-      <c r="D20" s="110" t="s">
+      <c r="C20" s="92">
+        <v>1</v>
+      </c>
+      <c r="D20" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="120" t="s">
+      <c r="E20" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="112" t="s">
+      <c r="F20" s="104" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="121" t="s">
+      <c r="G20" s="113" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="104" t="s">
+      <c r="H20" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="122" t="s">
+      <c r="I20" s="114" t="s">
         <v>88</v>
       </c>
-      <c r="J20" s="106" t="s">
+      <c r="J20" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="107">
+      <c r="K20" s="99">
         <v>1</v>
       </c>
       <c r="L20" s="53">
@@ -2130,31 +2091,31 @@
       <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="100">
+      <c r="C21" s="92">
         <v>2</v>
       </c>
-      <c r="D21" s="108" t="s">
+      <c r="D21" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="111" t="s">
+      <c r="E21" s="103" t="s">
         <v>107</v>
       </c>
-      <c r="F21" s="112" t="s">
+      <c r="F21" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="G21" s="113" t="s">
+      <c r="G21" s="105" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="104" t="s">
+      <c r="H21" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="96" t="s">
+      <c r="I21" s="90" t="s">
         <v>109</v>
       </c>
-      <c r="J21" s="106" t="s">
+      <c r="J21" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="107">
+      <c r="K21" s="99">
         <v>2</v>
       </c>
       <c r="L21" s="53">
@@ -2169,31 +2130,31 @@
       <c r="A22" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="100">
+      <c r="C22" s="92">
         <v>3</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="111" t="s">
+      <c r="E22" s="103" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="112" t="s">
+      <c r="F22" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="113" t="s">
+      <c r="G22" s="105" t="s">
         <v>77</v>
       </c>
-      <c r="H22" s="104" t="s">
+      <c r="H22" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="114" t="s">
+      <c r="I22" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="J22" s="106" t="s">
+      <c r="J22" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K22" s="107">
+      <c r="K22" s="99">
         <v>3</v>
       </c>
       <c r="L22" s="53">
@@ -2208,31 +2169,31 @@
       <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="100">
-        <v>1</v>
-      </c>
-      <c r="D23" s="108" t="s">
+      <c r="C23" s="92">
+        <v>1</v>
+      </c>
+      <c r="D23" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="111" t="s">
+      <c r="E23" s="103" t="s">
         <v>61</v>
       </c>
-      <c r="F23" s="112" t="s">
+      <c r="F23" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="G23" s="130" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="104" t="s">
+      <c r="G23" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="H23" s="96" t="s">
         <v>79</v>
       </c>
-      <c r="I23" s="130" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" s="106" t="s">
+      <c r="I23" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="J23" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="107">
+      <c r="K23" s="99">
         <v>1</v>
       </c>
       <c r="L23" s="53">
@@ -2247,31 +2208,31 @@
       <c r="A24" s="8">
         <v>1</v>
       </c>
-      <c r="C24" s="100">
+      <c r="C24" s="92">
         <v>2</v>
       </c>
-      <c r="D24" s="110" t="s">
+      <c r="D24" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="120" t="s">
+      <c r="E24" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="F24" s="112" t="s">
+      <c r="F24" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="121" t="s">
+      <c r="G24" s="113" t="s">
         <v>78</v>
       </c>
-      <c r="H24" s="104" t="s">
+      <c r="H24" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="122" t="s">
+      <c r="I24" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="J24" s="106" t="s">
+      <c r="J24" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="107">
+      <c r="K24" s="99">
         <v>2</v>
       </c>
       <c r="L24" s="53">
@@ -2286,29 +2247,29 @@
       <c r="A25" s="8">
         <v>1</v>
       </c>
-      <c r="C25" s="100">
-        <v>1</v>
-      </c>
-      <c r="D25" s="123"/>
-      <c r="E25" s="111" t="s">
+      <c r="C25" s="92">
+        <v>1</v>
+      </c>
+      <c r="D25" s="115"/>
+      <c r="E25" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="112" t="s">
+      <c r="F25" s="104" t="s">
         <v>69</v>
       </c>
-      <c r="G25" s="116" t="s">
+      <c r="G25" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="124" t="s">
+      <c r="H25" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="117" t="s">
+      <c r="I25" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="J25" s="106" t="s">
+      <c r="J25" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="107">
+      <c r="K25" s="99">
         <v>1</v>
       </c>
       <c r="L25" s="53"/>
@@ -2321,31 +2282,31 @@
       <c r="A26" s="8">
         <v>2</v>
       </c>
-      <c r="C26" s="100">
+      <c r="C26" s="92">
         <v>2</v>
       </c>
-      <c r="D26" s="108" t="s">
+      <c r="D26" s="100" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="120" t="s">
+      <c r="E26" s="112" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="121" t="s">
+      <c r="F26" s="113" t="s">
         <v>115</v>
       </c>
-      <c r="G26" s="95" t="s">
+      <c r="G26" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="H26" s="104" t="s">
+      <c r="H26" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="I26" s="96" t="s">
+      <c r="I26" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="J26" s="106" t="s">
+      <c r="J26" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="107">
+      <c r="K26" s="99">
         <v>2</v>
       </c>
       <c r="L26" s="53">
@@ -2360,46 +2321,46 @@
       <c r="A27" s="8">
         <v>1</v>
       </c>
-      <c r="C27" s="125" t="s">
+      <c r="C27" s="126" t="s">
         <v>102</v>
       </c>
-      <c r="D27" s="126"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="127"/>
-      <c r="H27" s="128"/>
-      <c r="I27" s="128"/>
-      <c r="J27" s="106"/>
-      <c r="K27" s="106"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="127"/>
+      <c r="F27" s="127"/>
+      <c r="G27" s="128"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="98"/>
       <c r="L27" s="53"/>
       <c r="M27" s="54"/>
     </row>
     <row r="28" spans="1:13" s="8" customFormat="1">
-      <c r="C28" s="100">
+      <c r="C28" s="92">
         <v>0</v>
       </c>
-      <c r="D28" s="101" t="s">
+      <c r="D28" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="E28" s="129" t="s">
+      <c r="E28" s="118" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="112" t="s">
+      <c r="F28" s="104" t="s">
         <v>97</v>
       </c>
-      <c r="G28" s="129" t="s">
+      <c r="G28" s="118" t="s">
         <v>98</v>
       </c>
-      <c r="H28" s="129" t="s">
+      <c r="H28" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="129" t="s">
+      <c r="I28" s="118" t="s">
         <v>100</v>
       </c>
-      <c r="J28" s="106" t="s">
+      <c r="J28" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="106">
+      <c r="K28" s="98">
         <v>0</v>
       </c>
       <c r="L28" s="53">
@@ -2414,31 +2375,31 @@
       <c r="A29" s="8">
         <v>1</v>
       </c>
-      <c r="C29" s="100">
+      <c r="C29" s="92">
         <v>0</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="109" t="s">
+      <c r="E29" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="112" t="s">
+      <c r="F29" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="G29" s="109" t="s">
+      <c r="G29" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="109" t="s">
+      <c r="H29" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="109" t="s">
+      <c r="I29" s="101" t="s">
         <v>101</v>
       </c>
-      <c r="J29" s="106" t="s">
+      <c r="J29" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="106">
+      <c r="K29" s="98">
         <v>0</v>
       </c>
       <c r="L29" s="53">
@@ -2522,8 +2483,8 @@
     <row r="34" spans="3:13" customFormat="1" ht="12.95" customHeight="1">
       <c r="C34" s="36"/>
       <c r="D34" s="30"/>
-      <c r="E34" s="99" t="s">
-        <v>120</v>
+      <c r="E34" s="91" t="s">
+        <v>117</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>

</xml_diff>

<commit_message>
Version 2.0, first draft, done and sent to PCB fab. Changed switches, crystal, USB connector, rerouted most of board. Still need to rename folder to 2.0
</commit_message>
<xml_diff>
--- a/mini/v17/Fubarino_Mini_v17_BOM_Microchip.xlsx
+++ b/mini/v17/Fubarino_Mini_v17_BOM_Microchip.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Brian\fubarino.github.com\mini\v17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\fubarino.github.com\mini\v17\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C45F8BA-2EF8-465D-AD01-45A3171350BD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23925" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23925" windowHeight="12045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
     <sheet name="Project Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="124">
   <si>
     <t>Approved</t>
   </si>
@@ -143,9 +144,6 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>IC1</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -179,30 +177,12 @@
     <t>D1, D2</t>
   </si>
   <si>
-    <t>CRYSTAL 8.00 MHZ 8PF SMD</t>
-  </si>
-  <si>
-    <t>CAP 1UF 10V CER Y5V SMD 0603</t>
-  </si>
-  <si>
     <t>CAP CER 10UF 10V Y5V 0805</t>
   </si>
   <si>
-    <t>CONN RECEPT MINI USB2.0 5POS</t>
-  </si>
-  <si>
-    <t>SWITCH TACT SMT SPST 160GF</t>
-  </si>
-  <si>
     <t>CAP CERAMIC .100UF 50V X7R 0603</t>
   </si>
   <si>
-    <t>LED SMARTLED 630NM RED 0603 SMD</t>
-  </si>
-  <si>
-    <t>LED SMARTLED GREEN 570NM 0603</t>
-  </si>
-  <si>
     <t>RES 10K OHM 1/10W 5% 0603 SMD</t>
   </si>
   <si>
@@ -212,9 +192,6 @@
     <t>CAP CER 12PF 50V 5% NP0 0603</t>
   </si>
   <si>
-    <t>NDK</t>
-  </si>
-  <si>
     <t>Microchip</t>
   </si>
   <si>
@@ -224,36 +201,18 @@
     <t>C&amp;K Components</t>
   </si>
   <si>
-    <t>OSRAM</t>
-  </si>
-  <si>
     <t>Panasonic</t>
   </si>
   <si>
     <t>???</t>
   </si>
   <si>
-    <t>NX5032GA 8MHZ AT-W</t>
-  </si>
-  <si>
-    <t>C0603C105Z8VACTU</t>
-  </si>
-  <si>
     <t>C2012Y5V1A106Z</t>
   </si>
   <si>
-    <t>PTS525SM10SMTR LFS</t>
-  </si>
-  <si>
     <t>C0603C104K5RACTU</t>
   </si>
   <si>
-    <t>LS L29K-G1J2-1-Z</t>
-  </si>
-  <si>
-    <t>LG L29K-G2J1-24-Z</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ103V</t>
   </si>
   <si>
@@ -269,27 +228,12 @@
     <t>Brian Schmalz</t>
   </si>
   <si>
-    <t>644-1132-1-ND</t>
-  </si>
-  <si>
-    <t>399-3216-1-ND</t>
-  </si>
-  <si>
     <t>445-1371-1-ND</t>
   </si>
   <si>
-    <t>CKN9104CT-ND</t>
-  </si>
-  <si>
     <t>399-5089-1-ND</t>
   </si>
   <si>
-    <t>475-2506-1-ND</t>
-  </si>
-  <si>
-    <t>475-2709-1-ND</t>
-  </si>
-  <si>
     <t>P10KGCT-ND</t>
   </si>
   <si>
@@ -332,15 +276,6 @@
     <t>DO NOT POPULATE ANY PARTS BELOW THIS LINE</t>
   </si>
   <si>
-    <t>Hirose</t>
-  </si>
-  <si>
-    <t>UX60-MB-5ST</t>
-  </si>
-  <si>
-    <t>H2959TR-ND</t>
-  </si>
-  <si>
     <t>02-10133r16.xls</t>
   </si>
   <si>
@@ -353,9 +288,6 @@
     <t>P820GCT-ND</t>
   </si>
   <si>
-    <t>Bill of Materials For Project Fubarino Mini v1.7</t>
-  </si>
-  <si>
     <t>Fubarino Mini v1.7 blank PCB</t>
   </si>
   <si>
@@ -371,28 +303,103 @@
     <t>Toshiba Semiconductor and Storage</t>
   </si>
   <si>
-    <t>Diodes Incorporated</t>
-  </si>
-  <si>
     <t>Parts changed from last production build</t>
   </si>
   <si>
     <t>PIC32MX270F256D-50I/ML  </t>
   </si>
   <si>
-    <t>AZ1117CR2-3.3TRG1-ND</t>
-  </si>
-  <si>
-    <t>AZ1117CR2-3.3TRG1</t>
-  </si>
-  <si>
-    <t>IC REG LINEAR 3.3V 800MA SOT89</t>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 800MA SOT223</t>
+  </si>
+  <si>
+    <t>MaxLinear, Inc.</t>
+  </si>
+  <si>
+    <t>SPX1117M3-L-3-3/TR</t>
+  </si>
+  <si>
+    <t>1016-1848-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 35V X5R 0603</t>
+  </si>
+  <si>
+    <t>Murata Electronics North America</t>
+  </si>
+  <si>
+    <t>GRM188R6YA475KE15D</t>
+  </si>
+  <si>
+    <t>490-7205-1-ND</t>
+  </si>
+  <si>
+    <t>Bill of Materials For Project Fubarino Mini v2.0</t>
+  </si>
+  <si>
+    <t>H125718CT-ND</t>
+  </si>
+  <si>
+    <t>Hirose Electric Co Ltd</t>
+  </si>
+  <si>
+    <t>ZX62D-B-5PA8(30)</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB MICRO B 2.0 5P SMD</t>
+  </si>
+  <si>
+    <t>LED RED CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>Lite-On Inc.</t>
+  </si>
+  <si>
+    <t>LTST-C193KRKT-5A</t>
+  </si>
+  <si>
+    <t>160-1830-1-ND</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>LTST-C193KGKT-5A</t>
+  </si>
+  <si>
+    <t>160-1828-1-ND</t>
+  </si>
+  <si>
+    <t>644-1178-1-ND</t>
+  </si>
+  <si>
+    <t>NDK America, Inc.</t>
+  </si>
+  <si>
+    <t>NX3225GD-8MHZ-STD-CRA-3</t>
+  </si>
+  <si>
+    <t>CRYSTAL 8.0000MHZ 8PF SMD</t>
+  </si>
+  <si>
+    <t>CKN10502DKR-ND</t>
+  </si>
+  <si>
+    <t>PTS810 SJM 250 SMTR LFS</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 16V</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
@@ -539,7 +546,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -857,6 +864,28 @@
       <top/>
       <bottom style="thin">
         <color indexed="62"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -874,7 +903,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1202,19 +1231,35 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 11" xfId="2"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 6" xfId="6"/>
-    <cellStyle name="Normal 7" xfId="7"/>
-    <cellStyle name="Normal 8" xfId="8"/>
-    <cellStyle name="Normal 9" xfId="9"/>
-    <cellStyle name="一般_MBT-9126_V1R1_BOM_060830" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 11" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 7" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 8" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 9" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="一般_MBT-9126_V1R1_BOM_060830" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1305,6 +1350,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1340,6 +1402,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1515,14 +1594,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1561,7 +1640,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="77" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1577,7 +1656,7 @@
         <v>24</v>
       </c>
       <c r="D3" s="74" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1594,7 +1673,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="75">
-        <v>1.7</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1611,7 +1690,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="76" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1628,7 +1707,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="76" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1737,30 +1816,30 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="8" customFormat="1">
+    <row r="12" spans="1:13" s="8" customFormat="1" ht="13.5" thickBot="1">
       <c r="A12" s="8">
         <v>4</v>
       </c>
       <c r="C12" s="92">
         <v>1</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="136" t="s">
         <v>39</v>
       </c>
       <c r="E12" s="94" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="F12" s="93" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="G12" s="95" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="H12" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I12" s="97" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="J12" s="98" t="s">
         <v>37</v>
@@ -1769,11 +1848,11 @@
         <v>1</v>
       </c>
       <c r="L12" s="53">
-        <v>1.7</v>
+        <v>0.94</v>
       </c>
       <c r="M12" s="54">
         <f t="shared" ref="M12:M29" si="0">K12*L12</f>
-        <v>1.7</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="8" customFormat="1">
@@ -1784,22 +1863,22 @@
         <v>1</v>
       </c>
       <c r="D13" s="100" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="90" t="s">
-        <v>121</v>
+        <v>95</v>
+      </c>
+      <c r="E13" s="129" t="s">
+        <v>96</v>
       </c>
       <c r="F13" s="101" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="G13" s="89" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="H13" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I13" s="90" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="J13" s="98" t="s">
         <v>37</v>
@@ -1808,10 +1887,11 @@
         <v>1</v>
       </c>
       <c r="L13" s="53">
-        <v>0.48</v>
+        <v>0.45</v>
       </c>
       <c r="M13" s="54">
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.45</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="8" customFormat="1">
@@ -1821,23 +1901,23 @@
       <c r="C14" s="92">
         <v>1</v>
       </c>
-      <c r="D14" s="102" t="s">
-        <v>41</v>
+      <c r="D14" s="100" t="s">
+        <v>40</v>
       </c>
       <c r="E14" s="103" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="F14" s="104" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="G14" s="105" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="H14" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="106" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="J14" s="98" t="s">
         <v>37</v>
@@ -1846,11 +1926,11 @@
         <v>1</v>
       </c>
       <c r="L14" s="53">
-        <v>0.1</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="M14" s="54">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="8" customFormat="1">
@@ -1861,22 +1941,22 @@
         <v>2</v>
       </c>
       <c r="D15" s="102" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="107" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F15" s="104" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G15" s="108" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="H15" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="109" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="J15" s="98" t="s">
         <v>37</v>
@@ -1899,17 +1979,17 @@
       <c r="C16" s="92">
         <v>1</v>
       </c>
-      <c r="D16" s="102" t="s">
-        <v>43</v>
+      <c r="D16" s="100" t="s">
+        <v>42</v>
       </c>
       <c r="E16" s="103" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="F16" s="104" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G16" s="110" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H16" s="96" t="s">
         <v>33</v>
@@ -1924,11 +2004,11 @@
         <v>1</v>
       </c>
       <c r="L16" s="53">
-        <v>0.52800000000000002</v>
+        <v>0.77</v>
       </c>
       <c r="M16" s="54">
         <f t="shared" si="0"/>
-        <v>0.52800000000000002</v>
+        <v>0.77</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="8" customFormat="1">
@@ -1938,23 +2018,23 @@
       <c r="C17" s="92">
         <v>2</v>
       </c>
-      <c r="D17" s="102" t="s">
-        <v>44</v>
+      <c r="D17" s="100" t="s">
+        <v>43</v>
       </c>
       <c r="E17" s="103" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="F17" s="104" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G17" s="105" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="H17" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I17" s="106" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="J17" s="98" t="s">
         <v>37</v>
@@ -1963,11 +2043,11 @@
         <v>2</v>
       </c>
       <c r="L17" s="53">
-        <v>0.61</v>
+        <v>0.3</v>
       </c>
       <c r="M17" s="54">
         <f t="shared" si="0"/>
-        <v>1.22</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="1:13" s="8" customFormat="1">
@@ -1978,22 +2058,22 @@
         <v>4</v>
       </c>
       <c r="D18" s="102" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E18" s="103" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="104" t="s">
-        <v>65</v>
-      </c>
       <c r="G18" s="105" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="H18" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I18" s="106" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="J18" s="98" t="s">
         <v>37</v>
@@ -2001,12 +2081,12 @@
       <c r="K18" s="99">
         <v>4</v>
       </c>
-      <c r="L18" s="53">
-        <v>0.1</v>
-      </c>
-      <c r="M18" s="54">
+      <c r="L18" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" s="54" t="e">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="8" customFormat="1">
@@ -2016,23 +2096,23 @@
       <c r="C19" s="92">
         <v>1</v>
       </c>
-      <c r="D19" s="102" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="112" t="s">
-        <v>58</v>
+      <c r="D19" s="100" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="103" t="s">
+        <v>109</v>
       </c>
       <c r="F19" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="G19" s="113" t="s">
-        <v>75</v>
-      </c>
-      <c r="H19" s="96" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" s="134" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="116" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="114" t="s">
-        <v>87</v>
+      <c r="I19" s="109" t="s">
+        <v>112</v>
       </c>
       <c r="J19" s="98" t="s">
         <v>37</v>
@@ -2041,11 +2121,11 @@
         <v>1</v>
       </c>
       <c r="L19" s="53">
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
       <c r="M19" s="54">
         <f>K19*L19</f>
-        <v>0.17</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="8" customFormat="1">
@@ -2055,23 +2135,23 @@
       <c r="C20" s="92">
         <v>1</v>
       </c>
-      <c r="D20" s="102" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="112" t="s">
-        <v>59</v>
+      <c r="D20" s="100" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="135" t="s">
+        <v>113</v>
       </c>
       <c r="F20" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="G20" s="113" t="s">
-        <v>76</v>
+        <v>110</v>
+      </c>
+      <c r="G20" s="130" t="s">
+        <v>114</v>
       </c>
       <c r="H20" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="114" t="s">
-        <v>88</v>
+      <c r="I20" s="135" t="s">
+        <v>115</v>
       </c>
       <c r="J20" s="98" t="s">
         <v>37</v>
@@ -2080,11 +2160,11 @@
         <v>1</v>
       </c>
       <c r="L20" s="53">
-        <v>0.22</v>
+        <v>0.15</v>
       </c>
       <c r="M20" s="54">
         <f t="shared" si="0"/>
-        <v>0.22</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="8" customFormat="1">
@@ -2095,22 +2175,22 @@
         <v>2</v>
       </c>
       <c r="D21" s="100" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="103" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="F21" s="104" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G21" s="105" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="H21" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I21" s="90" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="J21" s="98" t="s">
         <v>37</v>
@@ -2134,22 +2214,22 @@
         <v>3</v>
       </c>
       <c r="D22" s="102" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="103" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F22" s="104" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="G22" s="105" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="H22" s="96" t="s">
         <v>33</v>
       </c>
       <c r="I22" s="106" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="J22" s="98" t="s">
         <v>37</v>
@@ -2176,19 +2256,19 @@
         <v>28</v>
       </c>
       <c r="E23" s="103" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F23" s="104" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="119" t="s">
-        <v>118</v>
+        <v>56</v>
+      </c>
+      <c r="G23" s="133" t="s">
+        <v>94</v>
       </c>
       <c r="H23" s="96" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="I23" s="119" t="s">
-        <v>118</v>
+        <v>94</v>
       </c>
       <c r="J23" s="98" t="s">
         <v>37</v>
@@ -2212,22 +2292,22 @@
         <v>2</v>
       </c>
       <c r="D24" s="102" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E24" s="112" t="s">
-        <v>62</v>
-      </c>
-      <c r="F24" s="104" t="s">
-        <v>65</v>
+        <v>55</v>
+      </c>
+      <c r="F24" s="131" t="s">
+        <v>57</v>
       </c>
       <c r="G24" s="113" t="s">
-        <v>78</v>
-      </c>
-      <c r="H24" s="96" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24" s="132" t="s">
         <v>33</v>
       </c>
       <c r="I24" s="114" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="J24" s="98" t="s">
         <v>37</v>
@@ -2252,19 +2332,19 @@
       </c>
       <c r="D25" s="115"/>
       <c r="E25" s="103" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="F25" s="104" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G25" s="108" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="H25" s="116" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="I25" s="109" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="J25" s="98" t="s">
         <v>37</v>
@@ -2286,22 +2366,22 @@
         <v>2</v>
       </c>
       <c r="D26" s="100" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="112" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="113" t="s">
-        <v>115</v>
-      </c>
-      <c r="G26" s="89" t="s">
-        <v>112</v>
+        <v>91</v>
+      </c>
+      <c r="F26" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="G26" s="130" t="s">
+        <v>89</v>
       </c>
       <c r="H26" s="96" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="I26" s="90" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="J26" s="98" t="s">
         <v>37</v>
@@ -2322,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="126" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="D27" s="127"/>
       <c r="E27" s="127"/>
@@ -2340,22 +2420,22 @@
         <v>0</v>
       </c>
       <c r="D28" s="93" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="E28" s="118" t="s">
-        <v>94</v>
+        <v>75</v>
       </c>
       <c r="F28" s="104" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="G28" s="118" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="H28" s="118" t="s">
         <v>33</v>
       </c>
       <c r="I28" s="118" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="J28" s="98" t="s">
         <v>37</v>
@@ -2379,22 +2459,22 @@
         <v>0</v>
       </c>
       <c r="D29" s="93" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E29" s="101" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F29" s="104" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G29" s="101" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="H29" s="101" t="s">
         <v>33</v>
       </c>
       <c r="I29" s="101" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="J29" s="98" t="s">
         <v>37</v>
@@ -2418,10 +2498,10 @@
         <v>0</v>
       </c>
       <c r="D30" s="87" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E30" s="88" t="s">
-        <v>96</v>
+        <v>77</v>
       </c>
       <c r="F30" s="80"/>
       <c r="G30" s="80"/>
@@ -2443,9 +2523,9 @@
       <c r="J31" s="50"/>
       <c r="K31" s="50"/>
       <c r="L31" s="50"/>
-      <c r="M31" s="52">
+      <c r="M31" s="52" t="e">
         <f>SUM(M12:M30)</f>
-        <v>11.267999999999999</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
@@ -2484,7 +2564,7 @@
       <c r="C34" s="36"/>
       <c r="D34" s="30"/>
       <c r="E34" s="91" t="s">
-        <v>117</v>
+        <v>93</v>
       </c>
       <c r="F34" s="27"/>
       <c r="G34" s="27"/>
@@ -2589,7 +2669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>